<commit_message>
Gradle updated Daily scrums updated
</commit_message>
<xml_diff>
--- a/documents/DailyScrums.xlsx
+++ b/documents/DailyScrums.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chwu\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\Desktop\HTL\4BHIFS\FootballApp\FootballApp\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>1.Sprint</t>
   </si>
@@ -93,6 +93,21 @@
   </si>
   <si>
     <t>Grober Sprint Review</t>
+  </si>
+  <si>
+    <t>Sprintziel: Spieler anlegen, Spieler entfernen, Positionen verwalten, Spiel anlegen</t>
+  </si>
+  <si>
+    <t>Sprintplanung</t>
+  </si>
+  <si>
+    <t>Aufteilung der Aufgaben für das Wochenende</t>
+  </si>
+  <si>
+    <t>Besprechung aufgetretener Probleme</t>
+  </si>
+  <si>
+    <t>Planung der Akzeptanzkriterien und Testfälle</t>
   </si>
 </sst>
 </file>
@@ -222,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -231,11 +246,20 @@
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -247,13 +271,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -571,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,782 +600,746 @@
     <col min="7" max="7" width="17.140625" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" style="2"/>
     <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:35" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3">
         <v>42809</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="6" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="3">
         <v>42823</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="6" t="s">
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="P1" s="3">
         <v>42851</v>
       </c>
-      <c r="Q1" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="6" t="s">
+      <c r="Q1" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="W1" s="3">
         <v>42865</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="X1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
-      <c r="AA1" s="9"/>
-      <c r="AB1" s="9"/>
-      <c r="AC1" s="6" t="s">
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="AD1" s="3">
         <v>42879</v>
       </c>
-      <c r="AE1" s="9" t="s">
+      <c r="AE1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AF1" s="9"/>
-      <c r="AG1" s="9"/>
-      <c r="AH1" s="9"/>
-      <c r="AI1" s="9"/>
+      <c r="AF1" s="4"/>
+      <c r="AG1" s="4"/>
+      <c r="AH1" s="4"/>
+      <c r="AI1" s="4"/>
     </row>
     <row r="2" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5"/>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="5"/>
-      <c r="AC2" s="7"/>
-      <c r="AD2" s="4"/>
-      <c r="AE2" s="5"/>
-      <c r="AF2" s="5"/>
-      <c r="AG2" s="5"/>
-      <c r="AH2" s="5"/>
-      <c r="AI2" s="5"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="6"/>
+      <c r="AF2" s="6"/>
+      <c r="AG2" s="6"/>
+      <c r="AH2" s="6"/>
+      <c r="AI2" s="6"/>
     </row>
     <row r="3" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="1">
         <v>42810</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="H3" s="10"/>
       <c r="I3" s="1">
         <v>42844</v>
       </c>
       <c r="J3" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="7"/>
+      <c r="O3" s="10"/>
       <c r="P3" s="1">
         <v>42852</v>
       </c>
-      <c r="V3" s="7"/>
+      <c r="Q3" t="s">
+        <v>24</v>
+      </c>
+      <c r="V3" s="10"/>
       <c r="W3" s="1">
         <v>42866</v>
       </c>
-      <c r="AC3" s="7"/>
+      <c r="AC3" s="10"/>
       <c r="AD3" s="1">
         <v>42884</v>
       </c>
     </row>
     <row r="4" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="5"/>
-      <c r="Y4" s="5"/>
-      <c r="Z4" s="5"/>
-      <c r="AA4" s="5"/>
-      <c r="AB4" s="5"/>
-      <c r="AC4" s="7"/>
-      <c r="AD4" s="4"/>
-      <c r="AE4" s="5"/>
-      <c r="AF4" s="5"/>
-      <c r="AG4" s="5"/>
-      <c r="AH4" s="5"/>
-      <c r="AI4" s="5"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="10"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="6"/>
+      <c r="AI4" s="6"/>
     </row>
     <row r="5" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="1">
         <v>42811</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="7"/>
+      <c r="H5" s="10"/>
       <c r="I5" s="1">
         <v>42845</v>
       </c>
       <c r="J5" t="s">
         <v>8</v>
       </c>
-      <c r="O5" s="7"/>
+      <c r="O5" s="10"/>
       <c r="P5" s="1">
         <v>42853</v>
       </c>
-      <c r="V5" s="7"/>
+      <c r="Q5" t="s">
+        <v>25</v>
+      </c>
+      <c r="V5" s="10"/>
       <c r="W5" s="1">
         <v>42867</v>
       </c>
-      <c r="AC5" s="7"/>
+      <c r="AC5" s="10"/>
       <c r="AD5" s="1">
         <v>42885</v>
       </c>
     </row>
     <row r="6" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="4"/>
-      <c r="X6" s="5"/>
-      <c r="Y6" s="5"/>
-      <c r="Z6" s="5"/>
-      <c r="AA6" s="5"/>
-      <c r="AB6" s="5"/>
-      <c r="AC6" s="7"/>
-      <c r="AD6" s="4"/>
-      <c r="AE6" s="5"/>
-      <c r="AF6" s="5"/>
-      <c r="AG6" s="5"/>
-      <c r="AH6" s="5"/>
-      <c r="AI6" s="5"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="10"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="6"/>
+      <c r="AF6" s="6"/>
+      <c r="AG6" s="6"/>
+      <c r="AH6" s="6"/>
+      <c r="AI6" s="6"/>
     </row>
     <row r="7" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="1">
         <v>42814</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="7"/>
+      <c r="H7" s="10"/>
       <c r="I7" s="1">
         <v>42846</v>
       </c>
       <c r="J7" t="s">
         <v>11</v>
       </c>
-      <c r="O7" s="7"/>
+      <c r="O7" s="10"/>
       <c r="P7" s="1">
         <v>42857</v>
       </c>
-      <c r="V7" s="7"/>
+      <c r="Q7" t="s">
+        <v>26</v>
+      </c>
+      <c r="V7" s="10"/>
       <c r="W7" s="1">
         <v>42870</v>
       </c>
-      <c r="AC7" s="7"/>
+      <c r="AC7" s="10"/>
       <c r="AD7" s="1">
         <v>42886</v>
       </c>
     </row>
     <row r="8" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="5"/>
-      <c r="Y8" s="5"/>
-      <c r="Z8" s="5"/>
-      <c r="AA8" s="5"/>
-      <c r="AB8" s="5"/>
-      <c r="AC8" s="7"/>
-      <c r="AD8" s="4"/>
-      <c r="AE8" s="5"/>
-      <c r="AF8" s="5"/>
-      <c r="AG8" s="5"/>
-      <c r="AH8" s="5"/>
-      <c r="AI8" s="5"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="10"/>
+      <c r="AD8" s="5"/>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="6"/>
+      <c r="AG8" s="6"/>
+      <c r="AH8" s="6"/>
+      <c r="AI8" s="6"/>
     </row>
     <row r="9" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="1">
         <v>42815</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="7"/>
+      <c r="H9" s="10"/>
       <c r="I9" s="1">
         <v>42849</v>
       </c>
       <c r="J9" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="7"/>
+      <c r="O9" s="10"/>
       <c r="P9" s="1">
         <v>42858</v>
       </c>
-      <c r="V9" s="7"/>
+      <c r="Q9" t="s">
+        <v>27</v>
+      </c>
+      <c r="V9" s="10"/>
       <c r="W9" s="1">
         <v>42871</v>
       </c>
-      <c r="AC9" s="7"/>
+      <c r="AC9" s="10"/>
       <c r="AD9" s="1">
         <v>42887</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="7"/>
-      <c r="W10" s="4"/>
-      <c r="X10" s="5"/>
-      <c r="Y10" s="5"/>
-      <c r="Z10" s="5"/>
-      <c r="AA10" s="5"/>
-      <c r="AB10" s="5"/>
-      <c r="AC10" s="7"/>
-      <c r="AD10" s="4"/>
-      <c r="AE10" s="5"/>
-      <c r="AF10" s="5"/>
-      <c r="AG10" s="5"/>
-      <c r="AH10" s="5"/>
-      <c r="AI10" s="5"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="10"/>
+      <c r="AD10" s="5"/>
+      <c r="AE10" s="6"/>
+      <c r="AF10" s="6"/>
+      <c r="AG10" s="6"/>
+      <c r="AH10" s="6"/>
+      <c r="AI10" s="6"/>
     </row>
     <row r="11" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="1">
         <v>42816</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="7"/>
+      <c r="H11" s="10"/>
       <c r="I11" s="1">
         <v>42850</v>
       </c>
       <c r="J11" t="s">
         <v>10</v>
       </c>
-      <c r="O11" s="7"/>
+      <c r="O11" s="10"/>
       <c r="P11" s="1">
         <v>42859</v>
       </c>
-      <c r="V11" s="7"/>
+      <c r="V11" s="10"/>
       <c r="W11" s="1">
         <v>42872</v>
       </c>
-      <c r="AC11" s="7"/>
+      <c r="AC11" s="10"/>
       <c r="AD11" s="1">
         <v>42888</v>
       </c>
     </row>
     <row r="12" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
-      <c r="U12" s="5"/>
-      <c r="V12" s="7"/>
-      <c r="W12" s="4"/>
-      <c r="X12" s="5"/>
-      <c r="Y12" s="5"/>
-      <c r="Z12" s="5"/>
-      <c r="AA12" s="5"/>
-      <c r="AB12" s="5"/>
-      <c r="AC12" s="7"/>
-      <c r="AD12" s="4"/>
-      <c r="AE12" s="5"/>
-      <c r="AF12" s="5"/>
-      <c r="AG12" s="5"/>
-      <c r="AH12" s="5"/>
-      <c r="AI12" s="5"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
+      <c r="AA12" s="6"/>
+      <c r="AB12" s="6"/>
+      <c r="AC12" s="10"/>
+      <c r="AD12" s="5"/>
+      <c r="AE12" s="6"/>
+      <c r="AF12" s="6"/>
+      <c r="AG12" s="6"/>
+      <c r="AH12" s="6"/>
+      <c r="AI12" s="6"/>
     </row>
     <row r="13" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="1">
         <v>42817</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="7"/>
+      <c r="H13" s="10"/>
       <c r="I13" s="1"/>
-      <c r="O13" s="7"/>
+      <c r="O13" s="10"/>
       <c r="P13" s="1">
         <v>42860</v>
       </c>
-      <c r="V13" s="7"/>
+      <c r="V13" s="10"/>
       <c r="W13" s="1">
         <v>42873</v>
       </c>
-      <c r="AC13" s="7"/>
+      <c r="AC13" s="10"/>
       <c r="AD13" s="1">
         <v>42893</v>
       </c>
     </row>
     <row r="14" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="5"/>
-      <c r="U14" s="5"/>
-      <c r="V14" s="7"/>
-      <c r="W14" s="4"/>
-      <c r="X14" s="5"/>
-      <c r="Y14" s="5"/>
-      <c r="Z14" s="5"/>
-      <c r="AA14" s="5"/>
-      <c r="AB14" s="5"/>
-      <c r="AC14" s="7"/>
-      <c r="AD14" s="4"/>
-      <c r="AE14" s="5"/>
-      <c r="AF14" s="5"/>
-      <c r="AG14" s="5"/>
-      <c r="AH14" s="5"/>
-      <c r="AI14" s="5"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="6"/>
+      <c r="AA14" s="6"/>
+      <c r="AB14" s="6"/>
+      <c r="AC14" s="10"/>
+      <c r="AD14" s="5"/>
+      <c r="AE14" s="6"/>
+      <c r="AF14" s="6"/>
+      <c r="AG14" s="6"/>
+      <c r="AH14" s="6"/>
+      <c r="AI14" s="6"/>
     </row>
     <row r="15" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="1">
         <v>42818</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="7"/>
+      <c r="H15" s="10"/>
       <c r="I15" s="1"/>
-      <c r="O15" s="7"/>
+      <c r="O15" s="10"/>
       <c r="P15" s="1">
         <v>42863</v>
       </c>
-      <c r="V15" s="7"/>
+      <c r="V15" s="10"/>
       <c r="W15" s="1">
         <v>42874</v>
       </c>
-      <c r="AC15" s="7"/>
+      <c r="AC15" s="10"/>
       <c r="AD15" s="1">
         <v>42894</v>
       </c>
     </row>
     <row r="16" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
-      <c r="U16" s="5"/>
-      <c r="V16" s="7"/>
-      <c r="W16" s="4"/>
-      <c r="X16" s="5"/>
-      <c r="Y16" s="5"/>
-      <c r="Z16" s="5"/>
-      <c r="AA16" s="5"/>
-      <c r="AB16" s="5"/>
-      <c r="AC16" s="7"/>
-      <c r="AD16" s="4"/>
-      <c r="AE16" s="5"/>
-      <c r="AF16" s="5"/>
-      <c r="AG16" s="5"/>
-      <c r="AH16" s="5"/>
-      <c r="AI16" s="5"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="6"/>
+      <c r="AB16" s="6"/>
+      <c r="AC16" s="10"/>
+      <c r="AD16" s="5"/>
+      <c r="AE16" s="6"/>
+      <c r="AF16" s="6"/>
+      <c r="AG16" s="6"/>
+      <c r="AH16" s="6"/>
+      <c r="AI16" s="6"/>
     </row>
     <row r="17" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
+      <c r="A17" s="8"/>
       <c r="B17" s="1">
         <v>42821</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
       </c>
-      <c r="H17" s="7"/>
+      <c r="H17" s="10"/>
       <c r="I17" s="1"/>
-      <c r="O17" s="7"/>
+      <c r="O17" s="10"/>
       <c r="P17" s="1">
         <v>42864</v>
       </c>
-      <c r="V17" s="7"/>
+      <c r="V17" s="10"/>
       <c r="W17" s="1">
         <v>42877</v>
       </c>
-      <c r="AC17" s="7"/>
+      <c r="AC17" s="10"/>
       <c r="AD17" s="1">
         <v>42895</v>
       </c>
     </row>
     <row r="18" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
-      <c r="U18" s="5"/>
-      <c r="V18" s="7"/>
-      <c r="W18" s="4"/>
-      <c r="X18" s="5"/>
-      <c r="Y18" s="5"/>
-      <c r="Z18" s="5"/>
-      <c r="AA18" s="5"/>
-      <c r="AB18" s="5"/>
-      <c r="AC18" s="7"/>
-      <c r="AD18" s="4"/>
-      <c r="AE18" s="5"/>
-      <c r="AF18" s="5"/>
-      <c r="AG18" s="5"/>
-      <c r="AH18" s="5"/>
-      <c r="AI18" s="5"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="6"/>
+      <c r="AA18" s="6"/>
+      <c r="AB18" s="6"/>
+      <c r="AC18" s="10"/>
+      <c r="AD18" s="5"/>
+      <c r="AE18" s="6"/>
+      <c r="AF18" s="6"/>
+      <c r="AG18" s="6"/>
+      <c r="AH18" s="6"/>
+      <c r="AI18" s="6"/>
     </row>
     <row r="19" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
+      <c r="A19" s="8"/>
       <c r="B19" s="1">
         <v>42822</v>
       </c>
       <c r="C19" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="7"/>
+      <c r="H19" s="10"/>
       <c r="I19" s="1"/>
-      <c r="O19" s="7"/>
+      <c r="O19" s="10"/>
       <c r="P19" s="1"/>
-      <c r="V19" s="7"/>
+      <c r="V19" s="10"/>
       <c r="W19" s="1">
         <v>42878</v>
       </c>
-      <c r="AC19" s="7"/>
+      <c r="AC19" s="10"/>
       <c r="AD19" s="1">
         <v>42898</v>
       </c>
     </row>
     <row r="20" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="5"/>
-      <c r="T20" s="5"/>
-      <c r="U20" s="5"/>
-      <c r="V20" s="7"/>
-      <c r="W20" s="4"/>
-      <c r="X20" s="5"/>
-      <c r="Y20" s="5"/>
-      <c r="Z20" s="5"/>
-      <c r="AA20" s="5"/>
-      <c r="AB20" s="5"/>
-      <c r="AC20" s="7"/>
-      <c r="AD20" s="4"/>
-      <c r="AE20" s="5"/>
-      <c r="AF20" s="5"/>
-      <c r="AG20" s="5"/>
-      <c r="AH20" s="5"/>
-      <c r="AI20" s="5"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="10"/>
+      <c r="W20" s="5"/>
+      <c r="X20" s="6"/>
+      <c r="Y20" s="6"/>
+      <c r="Z20" s="6"/>
+      <c r="AA20" s="6"/>
+      <c r="AB20" s="6"/>
+      <c r="AC20" s="10"/>
+      <c r="AD20" s="5"/>
+      <c r="AE20" s="6"/>
+      <c r="AF20" s="6"/>
+      <c r="AG20" s="6"/>
+      <c r="AH20" s="6"/>
+      <c r="AI20" s="6"/>
     </row>
     <row r="21" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+      <c r="A21" s="8"/>
       <c r="B21" s="1">
         <v>42823</v>
       </c>
       <c r="C21" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="7"/>
+      <c r="H21" s="10"/>
       <c r="I21" s="1"/>
-      <c r="O21" s="7"/>
+      <c r="O21" s="10"/>
       <c r="P21" s="1"/>
-      <c r="V21" s="7"/>
+      <c r="V21" s="10"/>
       <c r="W21" s="1"/>
-      <c r="AC21" s="7"/>
+      <c r="AC21" s="10"/>
       <c r="AD21" s="1">
         <v>42899</v>
       </c>
     </row>
     <row r="22" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="5"/>
-      <c r="U22" s="5"/>
-      <c r="V22" s="8"/>
-      <c r="W22" s="4"/>
-      <c r="X22" s="5"/>
-      <c r="Y22" s="5"/>
-      <c r="Z22" s="5"/>
-      <c r="AA22" s="5"/>
-      <c r="AB22" s="5"/>
-      <c r="AC22" s="8"/>
-      <c r="AD22" s="4"/>
-      <c r="AE22" s="5"/>
-      <c r="AF22" s="5"/>
-      <c r="AG22" s="5"/>
-      <c r="AH22" s="5"/>
-      <c r="AI22" s="5"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="11"/>
+      <c r="W22" s="5"/>
+      <c r="X22" s="6"/>
+      <c r="Y22" s="6"/>
+      <c r="Z22" s="6"/>
+      <c r="AA22" s="6"/>
+      <c r="AB22" s="6"/>
+      <c r="AC22" s="11"/>
+      <c r="AD22" s="5"/>
+      <c r="AE22" s="6"/>
+      <c r="AF22" s="6"/>
+      <c r="AG22" s="6"/>
+      <c r="AH22" s="6"/>
+      <c r="AI22" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="I4:N4"/>
-    <mergeCell ref="I6:N6"/>
-    <mergeCell ref="I8:N8"/>
-    <mergeCell ref="A1:A22"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="H1:H22"/>
-    <mergeCell ref="I22:N22"/>
-    <mergeCell ref="O1:O22"/>
-    <mergeCell ref="Q1:U1"/>
-    <mergeCell ref="P2:U2"/>
-    <mergeCell ref="P4:U4"/>
-    <mergeCell ref="P6:U6"/>
-    <mergeCell ref="P8:U8"/>
-    <mergeCell ref="P10:U10"/>
-    <mergeCell ref="P12:U12"/>
-    <mergeCell ref="P14:U14"/>
-    <mergeCell ref="I10:N10"/>
-    <mergeCell ref="I12:N12"/>
-    <mergeCell ref="I14:N14"/>
-    <mergeCell ref="I16:N16"/>
-    <mergeCell ref="I18:N18"/>
-    <mergeCell ref="I20:N20"/>
-    <mergeCell ref="P22:U22"/>
-    <mergeCell ref="V1:V22"/>
-    <mergeCell ref="X1:AB1"/>
-    <mergeCell ref="W2:AB2"/>
-    <mergeCell ref="W4:AB4"/>
-    <mergeCell ref="W6:AB6"/>
-    <mergeCell ref="W8:AB8"/>
-    <mergeCell ref="W14:AB14"/>
-    <mergeCell ref="W16:AB16"/>
-    <mergeCell ref="W18:AB18"/>
-    <mergeCell ref="W20:AB20"/>
-    <mergeCell ref="P16:U16"/>
-    <mergeCell ref="P18:U18"/>
-    <mergeCell ref="P20:U20"/>
-    <mergeCell ref="J1:N1"/>
     <mergeCell ref="AD16:AI16"/>
     <mergeCell ref="AD18:AI18"/>
     <mergeCell ref="AD20:AI20"/>
@@ -1374,7 +1356,57 @@
     <mergeCell ref="AD14:AI14"/>
     <mergeCell ref="W10:AB10"/>
     <mergeCell ref="W12:AB12"/>
+    <mergeCell ref="V1:V22"/>
+    <mergeCell ref="X1:AB1"/>
+    <mergeCell ref="W2:AB2"/>
+    <mergeCell ref="W4:AB4"/>
+    <mergeCell ref="W6:AB6"/>
+    <mergeCell ref="W8:AB8"/>
+    <mergeCell ref="W14:AB14"/>
+    <mergeCell ref="W16:AB16"/>
+    <mergeCell ref="W18:AB18"/>
+    <mergeCell ref="W20:AB20"/>
+    <mergeCell ref="O1:O22"/>
+    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="P2:U2"/>
+    <mergeCell ref="P4:U4"/>
+    <mergeCell ref="P6:U6"/>
+    <mergeCell ref="P8:U8"/>
+    <mergeCell ref="P10:U10"/>
+    <mergeCell ref="P12:U12"/>
+    <mergeCell ref="P14:U14"/>
+    <mergeCell ref="P22:U22"/>
+    <mergeCell ref="P16:U16"/>
+    <mergeCell ref="P18:U18"/>
+    <mergeCell ref="P20:U20"/>
+    <mergeCell ref="A1:A22"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="I4:N4"/>
+    <mergeCell ref="I6:N6"/>
+    <mergeCell ref="I8:N8"/>
+    <mergeCell ref="H1:H22"/>
+    <mergeCell ref="I22:N22"/>
+    <mergeCell ref="I10:N10"/>
+    <mergeCell ref="I12:N12"/>
+    <mergeCell ref="I14:N14"/>
+    <mergeCell ref="I16:N16"/>
+    <mergeCell ref="I18:N18"/>
+    <mergeCell ref="I20:N20"/>
+    <mergeCell ref="J1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DailyScrums updated AddPlayerDialog added
</commit_message>
<xml_diff>
--- a/documents/DailyScrums.xlsx
+++ b/documents/DailyScrums.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>1.Sprint</t>
   </si>
@@ -108,6 +108,18 @@
   </si>
   <si>
     <t>Planung der Akzeptanzkriterien und Testfälle</t>
+  </si>
+  <si>
+    <t>Besprechung bezüglich "Spieler anlegen"</t>
+  </si>
+  <si>
+    <t>Besprechung Akzeptanzkriterien</t>
+  </si>
+  <si>
+    <t>Planung der Vorgehensweise aufgrund des Ausfalls von Wutti</t>
+  </si>
+  <si>
+    <t>Abschluss Akzeptanzkriterien</t>
   </si>
 </sst>
 </file>
@@ -246,20 +258,11 @@
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -271,7 +274,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -589,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20:U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,742 +616,803 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3">
         <v>42809</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="9" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="3">
         <v>42823</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="9" t="s">
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="P1" s="3">
         <v>42851</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="9" t="s">
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="W1" s="3">
         <v>42865</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="9" t="s">
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="AD1" s="3">
         <v>42879</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AE1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="AF1" s="4"/>
-      <c r="AG1" s="4"/>
-      <c r="AH1" s="4"/>
-      <c r="AI1" s="4"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
     </row>
     <row r="2" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="10"/>
-      <c r="AD2" s="5"/>
-      <c r="AE2" s="6"/>
-      <c r="AF2" s="6"/>
-      <c r="AG2" s="6"/>
-      <c r="AH2" s="6"/>
-      <c r="AI2" s="6"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="5"/>
+      <c r="AI2" s="5"/>
     </row>
     <row r="3" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="1">
         <v>42810</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="10"/>
+      <c r="H3" s="7"/>
       <c r="I3" s="1">
         <v>42844</v>
       </c>
       <c r="J3" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="10"/>
+      <c r="O3" s="7"/>
       <c r="P3" s="1">
         <v>42852</v>
       </c>
       <c r="Q3" t="s">
         <v>24</v>
       </c>
-      <c r="V3" s="10"/>
+      <c r="V3" s="7"/>
       <c r="W3" s="1">
         <v>42866</v>
       </c>
-      <c r="AC3" s="10"/>
+      <c r="AC3" s="7"/>
       <c r="AD3" s="1">
         <v>42884</v>
       </c>
     </row>
     <row r="4" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="5"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="6"/>
-      <c r="AA4" s="6"/>
-      <c r="AB4" s="6"/>
-      <c r="AC4" s="10"/>
-      <c r="AD4" s="5"/>
-      <c r="AE4" s="6"/>
-      <c r="AF4" s="6"/>
-      <c r="AG4" s="6"/>
-      <c r="AH4" s="6"/>
-      <c r="AI4" s="6"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="5"/>
+      <c r="AF4" s="5"/>
+      <c r="AG4" s="5"/>
+      <c r="AH4" s="5"/>
+      <c r="AI4" s="5"/>
     </row>
     <row r="5" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="1">
         <v>42811</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="10"/>
+      <c r="H5" s="7"/>
       <c r="I5" s="1">
         <v>42845</v>
       </c>
       <c r="J5" t="s">
         <v>8</v>
       </c>
-      <c r="O5" s="10"/>
+      <c r="O5" s="7"/>
       <c r="P5" s="1">
         <v>42853</v>
       </c>
       <c r="Q5" t="s">
         <v>25</v>
       </c>
-      <c r="V5" s="10"/>
+      <c r="V5" s="7"/>
       <c r="W5" s="1">
         <v>42867</v>
       </c>
-      <c r="AC5" s="10"/>
+      <c r="AC5" s="7"/>
       <c r="AD5" s="1">
         <v>42885</v>
       </c>
     </row>
     <row r="6" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="5"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-      <c r="Z6" s="6"/>
-      <c r="AA6" s="6"/>
-      <c r="AB6" s="6"/>
-      <c r="AC6" s="10"/>
-      <c r="AD6" s="5"/>
-      <c r="AE6" s="6"/>
-      <c r="AF6" s="6"/>
-      <c r="AG6" s="6"/>
-      <c r="AH6" s="6"/>
-      <c r="AI6" s="6"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="4"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="5"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="5"/>
+      <c r="AI6" s="5"/>
     </row>
     <row r="7" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="1">
         <v>42814</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="10"/>
+      <c r="H7" s="7"/>
       <c r="I7" s="1">
         <v>42846</v>
       </c>
       <c r="J7" t="s">
         <v>11</v>
       </c>
-      <c r="O7" s="10"/>
+      <c r="O7" s="7"/>
       <c r="P7" s="1">
         <v>42857</v>
       </c>
       <c r="Q7" t="s">
         <v>26</v>
       </c>
-      <c r="V7" s="10"/>
+      <c r="V7" s="7"/>
       <c r="W7" s="1">
         <v>42870</v>
       </c>
-      <c r="AC7" s="10"/>
+      <c r="AC7" s="7"/>
       <c r="AD7" s="1">
         <v>42886</v>
       </c>
     </row>
     <row r="8" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="10"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="6"/>
-      <c r="AA8" s="6"/>
-      <c r="AB8" s="6"/>
-      <c r="AC8" s="10"/>
-      <c r="AD8" s="5"/>
-      <c r="AE8" s="6"/>
-      <c r="AF8" s="6"/>
-      <c r="AG8" s="6"/>
-      <c r="AH8" s="6"/>
-      <c r="AI8" s="6"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="5"/>
+      <c r="AB8" s="5"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="4"/>
+      <c r="AE8" s="5"/>
+      <c r="AF8" s="5"/>
+      <c r="AG8" s="5"/>
+      <c r="AH8" s="5"/>
+      <c r="AI8" s="5"/>
     </row>
     <row r="9" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="1">
         <v>42815</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="10"/>
+      <c r="H9" s="7"/>
       <c r="I9" s="1">
         <v>42849</v>
       </c>
       <c r="J9" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="10"/>
+      <c r="O9" s="7"/>
       <c r="P9" s="1">
         <v>42858</v>
       </c>
       <c r="Q9" t="s">
         <v>27</v>
       </c>
-      <c r="V9" s="10"/>
+      <c r="V9" s="7"/>
       <c r="W9" s="1">
         <v>42871</v>
       </c>
-      <c r="AC9" s="10"/>
+      <c r="AC9" s="7"/>
       <c r="AD9" s="1">
         <v>42887</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6"/>
-      <c r="V10" s="10"/>
-      <c r="W10" s="5"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="6"/>
-      <c r="AA10" s="6"/>
-      <c r="AB10" s="6"/>
-      <c r="AC10" s="10"/>
-      <c r="AD10" s="5"/>
-      <c r="AE10" s="6"/>
-      <c r="AF10" s="6"/>
-      <c r="AG10" s="6"/>
-      <c r="AH10" s="6"/>
-      <c r="AI10" s="6"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="5"/>
+      <c r="AB10" s="5"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="4"/>
+      <c r="AE10" s="5"/>
+      <c r="AF10" s="5"/>
+      <c r="AG10" s="5"/>
+      <c r="AH10" s="5"/>
+      <c r="AI10" s="5"/>
     </row>
     <row r="11" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="1">
         <v>42816</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="10"/>
+      <c r="H11" s="7"/>
       <c r="I11" s="1">
         <v>42850</v>
       </c>
       <c r="J11" t="s">
         <v>10</v>
       </c>
-      <c r="O11" s="10"/>
+      <c r="O11" s="7"/>
       <c r="P11" s="1">
         <v>42859</v>
       </c>
-      <c r="V11" s="10"/>
+      <c r="Q11" t="s">
+        <v>28</v>
+      </c>
+      <c r="V11" s="7"/>
       <c r="W11" s="1">
         <v>42872</v>
       </c>
-      <c r="AC11" s="10"/>
+      <c r="AC11" s="7"/>
       <c r="AD11" s="1">
         <v>42888</v>
       </c>
     </row>
     <row r="12" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="10"/>
-      <c r="W12" s="5"/>
-      <c r="X12" s="6"/>
-      <c r="Y12" s="6"/>
-      <c r="Z12" s="6"/>
-      <c r="AA12" s="6"/>
-      <c r="AB12" s="6"/>
-      <c r="AC12" s="10"/>
-      <c r="AD12" s="5"/>
-      <c r="AE12" s="6"/>
-      <c r="AF12" s="6"/>
-      <c r="AG12" s="6"/>
-      <c r="AH12" s="6"/>
-      <c r="AI12" s="6"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="5"/>
+      <c r="AB12" s="5"/>
+      <c r="AC12" s="7"/>
+      <c r="AD12" s="4"/>
+      <c r="AE12" s="5"/>
+      <c r="AF12" s="5"/>
+      <c r="AG12" s="5"/>
+      <c r="AH12" s="5"/>
+      <c r="AI12" s="5"/>
     </row>
     <row r="13" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="1">
         <v>42817</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="10"/>
+      <c r="H13" s="7"/>
       <c r="I13" s="1"/>
-      <c r="O13" s="10"/>
+      <c r="O13" s="7"/>
       <c r="P13" s="1">
         <v>42860</v>
       </c>
-      <c r="V13" s="10"/>
+      <c r="Q13" t="s">
+        <v>29</v>
+      </c>
+      <c r="V13" s="7"/>
       <c r="W13" s="1">
         <v>42873</v>
       </c>
-      <c r="AC13" s="10"/>
+      <c r="AC13" s="7"/>
       <c r="AD13" s="1">
         <v>42893</v>
       </c>
     </row>
     <row r="14" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
-      <c r="V14" s="10"/>
-      <c r="W14" s="5"/>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="6"/>
-      <c r="Z14" s="6"/>
-      <c r="AA14" s="6"/>
-      <c r="AB14" s="6"/>
-      <c r="AC14" s="10"/>
-      <c r="AD14" s="5"/>
-      <c r="AE14" s="6"/>
-      <c r="AF14" s="6"/>
-      <c r="AG14" s="6"/>
-      <c r="AH14" s="6"/>
-      <c r="AI14" s="6"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="5"/>
+      <c r="AC14" s="7"/>
+      <c r="AD14" s="4"/>
+      <c r="AE14" s="5"/>
+      <c r="AF14" s="5"/>
+      <c r="AG14" s="5"/>
+      <c r="AH14" s="5"/>
+      <c r="AI14" s="5"/>
     </row>
     <row r="15" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="1">
         <v>42818</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="10"/>
+      <c r="H15" s="7"/>
       <c r="I15" s="1"/>
-      <c r="O15" s="10"/>
+      <c r="O15" s="7"/>
       <c r="P15" s="1">
         <v>42863</v>
       </c>
-      <c r="V15" s="10"/>
+      <c r="Q15" t="s">
+        <v>30</v>
+      </c>
+      <c r="V15" s="7"/>
       <c r="W15" s="1">
         <v>42874</v>
       </c>
-      <c r="AC15" s="10"/>
+      <c r="AC15" s="7"/>
       <c r="AD15" s="1">
         <v>42894</v>
       </c>
     </row>
     <row r="16" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
-      <c r="S16" s="6"/>
-      <c r="T16" s="6"/>
-      <c r="U16" s="6"/>
-      <c r="V16" s="10"/>
-      <c r="W16" s="5"/>
-      <c r="X16" s="6"/>
-      <c r="Y16" s="6"/>
-      <c r="Z16" s="6"/>
-      <c r="AA16" s="6"/>
-      <c r="AB16" s="6"/>
-      <c r="AC16" s="10"/>
-      <c r="AD16" s="5"/>
-      <c r="AE16" s="6"/>
-      <c r="AF16" s="6"/>
-      <c r="AG16" s="6"/>
-      <c r="AH16" s="6"/>
-      <c r="AI16" s="6"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="4"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="5"/>
+      <c r="Z16" s="5"/>
+      <c r="AA16" s="5"/>
+      <c r="AB16" s="5"/>
+      <c r="AC16" s="7"/>
+      <c r="AD16" s="4"/>
+      <c r="AE16" s="5"/>
+      <c r="AF16" s="5"/>
+      <c r="AG16" s="5"/>
+      <c r="AH16" s="5"/>
+      <c r="AI16" s="5"/>
     </row>
     <row r="17" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="1">
         <v>42821</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
       </c>
-      <c r="H17" s="10"/>
+      <c r="H17" s="7"/>
       <c r="I17" s="1"/>
-      <c r="O17" s="10"/>
+      <c r="O17" s="7"/>
       <c r="P17" s="1">
         <v>42864</v>
       </c>
-      <c r="V17" s="10"/>
+      <c r="Q17" t="s">
+        <v>31</v>
+      </c>
+      <c r="V17" s="7"/>
       <c r="W17" s="1">
         <v>42877</v>
       </c>
-      <c r="AC17" s="10"/>
+      <c r="AC17" s="7"/>
       <c r="AD17" s="1">
         <v>42895</v>
       </c>
     </row>
     <row r="18" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
-      <c r="S18" s="6"/>
-      <c r="T18" s="6"/>
-      <c r="U18" s="6"/>
-      <c r="V18" s="10"/>
-      <c r="W18" s="5"/>
-      <c r="X18" s="6"/>
-      <c r="Y18" s="6"/>
-      <c r="Z18" s="6"/>
-      <c r="AA18" s="6"/>
-      <c r="AB18" s="6"/>
-      <c r="AC18" s="10"/>
-      <c r="AD18" s="5"/>
-      <c r="AE18" s="6"/>
-      <c r="AF18" s="6"/>
-      <c r="AG18" s="6"/>
-      <c r="AH18" s="6"/>
-      <c r="AI18" s="6"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="5"/>
+      <c r="AB18" s="5"/>
+      <c r="AC18" s="7"/>
+      <c r="AD18" s="4"/>
+      <c r="AE18" s="5"/>
+      <c r="AF18" s="5"/>
+      <c r="AG18" s="5"/>
+      <c r="AH18" s="5"/>
+      <c r="AI18" s="5"/>
     </row>
     <row r="19" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="1">
         <v>42822</v>
       </c>
       <c r="C19" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="10"/>
+      <c r="H19" s="7"/>
       <c r="I19" s="1"/>
-      <c r="O19" s="10"/>
+      <c r="O19" s="7"/>
       <c r="P19" s="1"/>
-      <c r="V19" s="10"/>
+      <c r="V19" s="7"/>
       <c r="W19" s="1">
         <v>42878</v>
       </c>
-      <c r="AC19" s="10"/>
+      <c r="AC19" s="7"/>
       <c r="AD19" s="1">
         <v>42898</v>
       </c>
     </row>
     <row r="20" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6"/>
-      <c r="U20" s="6"/>
-      <c r="V20" s="10"/>
-      <c r="W20" s="5"/>
-      <c r="X20" s="6"/>
-      <c r="Y20" s="6"/>
-      <c r="Z20" s="6"/>
-      <c r="AA20" s="6"/>
-      <c r="AB20" s="6"/>
-      <c r="AC20" s="10"/>
-      <c r="AD20" s="5"/>
-      <c r="AE20" s="6"/>
-      <c r="AF20" s="6"/>
-      <c r="AG20" s="6"/>
-      <c r="AH20" s="6"/>
-      <c r="AI20" s="6"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="4"/>
+      <c r="X20" s="5"/>
+      <c r="Y20" s="5"/>
+      <c r="Z20" s="5"/>
+      <c r="AA20" s="5"/>
+      <c r="AB20" s="5"/>
+      <c r="AC20" s="7"/>
+      <c r="AD20" s="4"/>
+      <c r="AE20" s="5"/>
+      <c r="AF20" s="5"/>
+      <c r="AG20" s="5"/>
+      <c r="AH20" s="5"/>
+      <c r="AI20" s="5"/>
     </row>
     <row r="21" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="1">
         <v>42823</v>
       </c>
       <c r="C21" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="10"/>
+      <c r="H21" s="7"/>
       <c r="I21" s="1"/>
-      <c r="O21" s="10"/>
+      <c r="O21" s="7"/>
       <c r="P21" s="1"/>
-      <c r="V21" s="10"/>
+      <c r="V21" s="7"/>
       <c r="W21" s="1"/>
-      <c r="AC21" s="10"/>
+      <c r="AC21" s="7"/>
       <c r="AD21" s="1">
         <v>42899</v>
       </c>
     </row>
     <row r="22" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="11"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="6"/>
-      <c r="S22" s="6"/>
-      <c r="T22" s="6"/>
-      <c r="U22" s="6"/>
-      <c r="V22" s="11"/>
-      <c r="W22" s="5"/>
-      <c r="X22" s="6"/>
-      <c r="Y22" s="6"/>
-      <c r="Z22" s="6"/>
-      <c r="AA22" s="6"/>
-      <c r="AB22" s="6"/>
-      <c r="AC22" s="11"/>
-      <c r="AD22" s="5"/>
-      <c r="AE22" s="6"/>
-      <c r="AF22" s="6"/>
-      <c r="AG22" s="6"/>
-      <c r="AH22" s="6"/>
-      <c r="AI22" s="6"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="5"/>
+      <c r="V22" s="8"/>
+      <c r="W22" s="4"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="5"/>
+      <c r="Z22" s="5"/>
+      <c r="AA22" s="5"/>
+      <c r="AB22" s="5"/>
+      <c r="AC22" s="8"/>
+      <c r="AD22" s="4"/>
+      <c r="AE22" s="5"/>
+      <c r="AF22" s="5"/>
+      <c r="AG22" s="5"/>
+      <c r="AH22" s="5"/>
+      <c r="AI22" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="65">
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="I4:N4"/>
+    <mergeCell ref="I6:N6"/>
+    <mergeCell ref="I8:N8"/>
+    <mergeCell ref="H1:H22"/>
+    <mergeCell ref="I22:N22"/>
+    <mergeCell ref="I10:N10"/>
+    <mergeCell ref="I12:N12"/>
+    <mergeCell ref="I14:N14"/>
+    <mergeCell ref="I16:N16"/>
+    <mergeCell ref="I18:N18"/>
+    <mergeCell ref="I20:N20"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="A1:A22"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="O1:O22"/>
+    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="P2:U2"/>
+    <mergeCell ref="P4:U4"/>
+    <mergeCell ref="P6:U6"/>
+    <mergeCell ref="P8:U8"/>
+    <mergeCell ref="P10:U10"/>
+    <mergeCell ref="P12:U12"/>
+    <mergeCell ref="P14:U14"/>
+    <mergeCell ref="P22:U22"/>
+    <mergeCell ref="P16:U16"/>
+    <mergeCell ref="P18:U18"/>
+    <mergeCell ref="P20:U20"/>
+    <mergeCell ref="V1:V22"/>
+    <mergeCell ref="X1:AB1"/>
+    <mergeCell ref="W2:AB2"/>
+    <mergeCell ref="W4:AB4"/>
+    <mergeCell ref="W6:AB6"/>
+    <mergeCell ref="W8:AB8"/>
+    <mergeCell ref="W14:AB14"/>
+    <mergeCell ref="W16:AB16"/>
+    <mergeCell ref="W18:AB18"/>
+    <mergeCell ref="W20:AB20"/>
     <mergeCell ref="AD16:AI16"/>
     <mergeCell ref="AD18:AI18"/>
     <mergeCell ref="AD20:AI20"/>
@@ -1356,55 +1429,6 @@
     <mergeCell ref="AD14:AI14"/>
     <mergeCell ref="W10:AB10"/>
     <mergeCell ref="W12:AB12"/>
-    <mergeCell ref="V1:V22"/>
-    <mergeCell ref="X1:AB1"/>
-    <mergeCell ref="W2:AB2"/>
-    <mergeCell ref="W4:AB4"/>
-    <mergeCell ref="W6:AB6"/>
-    <mergeCell ref="W8:AB8"/>
-    <mergeCell ref="W14:AB14"/>
-    <mergeCell ref="W16:AB16"/>
-    <mergeCell ref="W18:AB18"/>
-    <mergeCell ref="W20:AB20"/>
-    <mergeCell ref="O1:O22"/>
-    <mergeCell ref="Q1:U1"/>
-    <mergeCell ref="P2:U2"/>
-    <mergeCell ref="P4:U4"/>
-    <mergeCell ref="P6:U6"/>
-    <mergeCell ref="P8:U8"/>
-    <mergeCell ref="P10:U10"/>
-    <mergeCell ref="P12:U12"/>
-    <mergeCell ref="P14:U14"/>
-    <mergeCell ref="P22:U22"/>
-    <mergeCell ref="P16:U16"/>
-    <mergeCell ref="P18:U18"/>
-    <mergeCell ref="P20:U20"/>
-    <mergeCell ref="A1:A22"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="I4:N4"/>
-    <mergeCell ref="I6:N6"/>
-    <mergeCell ref="I8:N8"/>
-    <mergeCell ref="H1:H22"/>
-    <mergeCell ref="I22:N22"/>
-    <mergeCell ref="I10:N10"/>
-    <mergeCell ref="I12:N12"/>
-    <mergeCell ref="I14:N14"/>
-    <mergeCell ref="I16:N16"/>
-    <mergeCell ref="I18:N18"/>
-    <mergeCell ref="I20:N20"/>
-    <mergeCell ref="J1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
GetAllPlayers added (not working correctly) DailyScrums
</commit_message>
<xml_diff>
--- a/documents/DailyScrums.xlsx
+++ b/documents/DailyScrums.xlsx
@@ -95,9 +95,6 @@
     <t>Grober Sprint Review</t>
   </si>
   <si>
-    <t>Sprintziel: Spieler anlegen, Spieler entfernen, Positionen verwalten, Spiel anlegen</t>
-  </si>
-  <si>
     <t>Sprintplanung</t>
   </si>
   <si>
@@ -120,6 +117,9 @@
   </si>
   <si>
     <t>Abschluss Akzeptanzkriterien</t>
+  </si>
+  <si>
+    <t>Sprintziel: Spieler anlegen, Spieler entfernen, Spiel anlegen</t>
   </si>
 </sst>
 </file>
@@ -276,14 +276,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -602,7 +602,7 @@
   <dimension ref="A1:AI22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20:U20"/>
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,7 +616,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3">
@@ -648,13 +648,13 @@
       <c r="P1" s="3">
         <v>42851</v>
       </c>
-      <c r="Q1" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
+      <c r="Q1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
       <c r="V1" s="6" t="s">
         <v>4</v>
       </c>
@@ -683,7 +683,7 @@
       <c r="AI1" s="9"/>
     </row>
     <row r="2" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
+      <c r="A2" s="11"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -720,7 +720,7 @@
       <c r="AI2" s="5"/>
     </row>
     <row r="3" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="1">
         <v>42810</v>
       </c>
@@ -739,7 +739,7 @@
         <v>42852</v>
       </c>
       <c r="Q3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="V3" s="7"/>
       <c r="W3" s="1">
@@ -751,7 +751,7 @@
       </c>
     </row>
     <row r="4" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -788,7 +788,7 @@
       <c r="AI4" s="5"/>
     </row>
     <row r="5" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
+      <c r="A5" s="11"/>
       <c r="B5" s="1">
         <v>42811</v>
       </c>
@@ -807,7 +807,7 @@
         <v>42853</v>
       </c>
       <c r="Q5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="V5" s="7"/>
       <c r="W5" s="1">
@@ -819,7 +819,7 @@
       </c>
     </row>
     <row r="6" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -856,7 +856,7 @@
       <c r="AI6" s="5"/>
     </row>
     <row r="7" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="1">
         <v>42814</v>
       </c>
@@ -875,7 +875,7 @@
         <v>42857</v>
       </c>
       <c r="Q7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="V7" s="7"/>
       <c r="W7" s="1">
@@ -887,7 +887,7 @@
       </c>
     </row>
     <row r="8" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -924,7 +924,7 @@
       <c r="AI8" s="5"/>
     </row>
     <row r="9" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="1">
         <v>42815</v>
       </c>
@@ -943,7 +943,7 @@
         <v>42858</v>
       </c>
       <c r="Q9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V9" s="7"/>
       <c r="W9" s="1">
@@ -955,7 +955,7 @@
       </c>
     </row>
     <row r="10" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -992,7 +992,7 @@
       <c r="AI10" s="5"/>
     </row>
     <row r="11" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="1">
         <v>42816</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>42859</v>
       </c>
       <c r="Q11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V11" s="7"/>
       <c r="W11" s="1">
@@ -1023,7 +1023,7 @@
       </c>
     </row>
     <row r="12" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1060,7 +1060,7 @@
       <c r="AI12" s="5"/>
     </row>
     <row r="13" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="1">
         <v>42817</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>42860</v>
       </c>
       <c r="Q13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="V13" s="7"/>
       <c r="W13" s="1">
@@ -1086,7 +1086,7 @@
       </c>
     </row>
     <row r="14" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1123,7 +1123,7 @@
       <c r="AI14" s="5"/>
     </row>
     <row r="15" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="1">
         <v>42818</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>42863</v>
       </c>
       <c r="Q15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="V15" s="7"/>
       <c r="W15" s="1">
@@ -1149,7 +1149,7 @@
       </c>
     </row>
     <row r="16" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -1186,7 +1186,7 @@
       <c r="AI16" s="5"/>
     </row>
     <row r="17" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="1">
         <v>42821</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>42864</v>
       </c>
       <c r="Q17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V17" s="7"/>
       <c r="W17" s="1">
@@ -1212,7 +1212,7 @@
       </c>
     </row>
     <row r="18" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1249,7 +1249,7 @@
       <c r="AI18" s="5"/>
     </row>
     <row r="19" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="1">
         <v>42822</v>
       </c>
@@ -1270,7 +1270,7 @@
       </c>
     </row>
     <row r="20" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -1307,7 +1307,7 @@
       <c r="AI20" s="5"/>
     </row>
     <row r="21" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="1">
         <v>42823</v>
       </c>
@@ -1326,7 +1326,7 @@
       </c>
     </row>
     <row r="22" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -1364,55 +1364,6 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="I4:N4"/>
-    <mergeCell ref="I6:N6"/>
-    <mergeCell ref="I8:N8"/>
-    <mergeCell ref="H1:H22"/>
-    <mergeCell ref="I22:N22"/>
-    <mergeCell ref="I10:N10"/>
-    <mergeCell ref="I12:N12"/>
-    <mergeCell ref="I14:N14"/>
-    <mergeCell ref="I16:N16"/>
-    <mergeCell ref="I18:N18"/>
-    <mergeCell ref="I20:N20"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="A1:A22"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="O1:O22"/>
-    <mergeCell ref="Q1:U1"/>
-    <mergeCell ref="P2:U2"/>
-    <mergeCell ref="P4:U4"/>
-    <mergeCell ref="P6:U6"/>
-    <mergeCell ref="P8:U8"/>
-    <mergeCell ref="P10:U10"/>
-    <mergeCell ref="P12:U12"/>
-    <mergeCell ref="P14:U14"/>
-    <mergeCell ref="P22:U22"/>
-    <mergeCell ref="P16:U16"/>
-    <mergeCell ref="P18:U18"/>
-    <mergeCell ref="P20:U20"/>
-    <mergeCell ref="V1:V22"/>
-    <mergeCell ref="X1:AB1"/>
-    <mergeCell ref="W2:AB2"/>
-    <mergeCell ref="W4:AB4"/>
-    <mergeCell ref="W6:AB6"/>
-    <mergeCell ref="W8:AB8"/>
-    <mergeCell ref="W14:AB14"/>
-    <mergeCell ref="W16:AB16"/>
-    <mergeCell ref="W18:AB18"/>
-    <mergeCell ref="W20:AB20"/>
     <mergeCell ref="AD16:AI16"/>
     <mergeCell ref="AD18:AI18"/>
     <mergeCell ref="AD20:AI20"/>
@@ -1429,6 +1380,55 @@
     <mergeCell ref="AD14:AI14"/>
     <mergeCell ref="W10:AB10"/>
     <mergeCell ref="W12:AB12"/>
+    <mergeCell ref="V1:V22"/>
+    <mergeCell ref="X1:AB1"/>
+    <mergeCell ref="W2:AB2"/>
+    <mergeCell ref="W4:AB4"/>
+    <mergeCell ref="W6:AB6"/>
+    <mergeCell ref="W8:AB8"/>
+    <mergeCell ref="W14:AB14"/>
+    <mergeCell ref="W16:AB16"/>
+    <mergeCell ref="W18:AB18"/>
+    <mergeCell ref="W20:AB20"/>
+    <mergeCell ref="O1:O22"/>
+    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="P2:U2"/>
+    <mergeCell ref="P4:U4"/>
+    <mergeCell ref="P6:U6"/>
+    <mergeCell ref="P8:U8"/>
+    <mergeCell ref="P10:U10"/>
+    <mergeCell ref="P12:U12"/>
+    <mergeCell ref="P14:U14"/>
+    <mergeCell ref="P22:U22"/>
+    <mergeCell ref="P16:U16"/>
+    <mergeCell ref="P18:U18"/>
+    <mergeCell ref="P20:U20"/>
+    <mergeCell ref="A1:A22"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="I4:N4"/>
+    <mergeCell ref="I6:N6"/>
+    <mergeCell ref="I8:N8"/>
+    <mergeCell ref="H1:H22"/>
+    <mergeCell ref="I22:N22"/>
+    <mergeCell ref="I10:N10"/>
+    <mergeCell ref="I12:N12"/>
+    <mergeCell ref="I14:N14"/>
+    <mergeCell ref="I16:N16"/>
+    <mergeCell ref="I18:N18"/>
+    <mergeCell ref="I20:N20"/>
+    <mergeCell ref="J1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Occupations added Daily Scrums updated
</commit_message>
<xml_diff>
--- a/documents/DailyScrums.xlsx
+++ b/documents/DailyScrums.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>1.Sprint</t>
   </si>
@@ -119,7 +119,28 @@
     <t>Abschluss Akzeptanzkriterien</t>
   </si>
   <si>
-    <t>Sprintziel: Spieler anlegen, Spieler entfernen, Spiel anlegen</t>
+    <t>Sprintziel: Spieler anlegen, Vorarbeiten zu Spieler entfernen</t>
+  </si>
+  <si>
+    <t>Planung zur weiteren Vorgehensweise</t>
+  </si>
+  <si>
+    <t>Sprintziel: Spieler entfernen, Spiel anlegen, Positionsverwaltung, Login</t>
+  </si>
+  <si>
+    <t>Besprechung zu Spieler entfernen</t>
+  </si>
+  <si>
+    <t>Besprechung zur Positionsverwaltung</t>
+  </si>
+  <si>
+    <t>Besprechung zu Login und Spiel anlegen</t>
+  </si>
+  <si>
+    <t>Planung zur Präsentation für 23.5.</t>
+  </si>
+  <si>
+    <t>Sprint Review</t>
   </si>
 </sst>
 </file>
@@ -601,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AG13" sqref="AG13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,6 +634,7 @@
     <col min="8" max="8" width="11.42578125" style="2"/>
     <col min="9" max="9" width="14.5703125" customWidth="1"/>
     <col min="17" max="17" width="11.42578125" customWidth="1"/>
+    <col min="28" max="28" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -662,7 +684,7 @@
         <v>42865</v>
       </c>
       <c r="X1" s="9" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="Y1" s="9"/>
       <c r="Z1" s="9"/>
@@ -745,6 +767,9 @@
       <c r="W3" s="1">
         <v>42866</v>
       </c>
+      <c r="X3" t="s">
+        <v>23</v>
+      </c>
       <c r="AC3" s="7"/>
       <c r="AD3" s="1">
         <v>42884</v>
@@ -813,6 +838,9 @@
       <c r="W5" s="1">
         <v>42867</v>
       </c>
+      <c r="X5" t="s">
+        <v>32</v>
+      </c>
       <c r="AC5" s="7"/>
       <c r="AD5" s="1">
         <v>42885</v>
@@ -881,6 +909,9 @@
       <c r="W7" s="1">
         <v>42870</v>
       </c>
+      <c r="X7" t="s">
+        <v>34</v>
+      </c>
       <c r="AC7" s="7"/>
       <c r="AD7" s="1">
         <v>42886</v>
@@ -949,6 +980,9 @@
       <c r="W9" s="1">
         <v>42871</v>
       </c>
+      <c r="X9" t="s">
+        <v>35</v>
+      </c>
       <c r="AC9" s="7"/>
       <c r="AD9" s="1">
         <v>42887</v>
@@ -1017,6 +1051,9 @@
       <c r="W11" s="1">
         <v>42872</v>
       </c>
+      <c r="X11" t="s">
+        <v>36</v>
+      </c>
       <c r="AC11" s="7"/>
       <c r="AD11" s="1">
         <v>42888</v>
@@ -1080,6 +1117,9 @@
       <c r="W13" s="1">
         <v>42873</v>
       </c>
+      <c r="X13" t="s">
+        <v>28</v>
+      </c>
       <c r="AC13" s="7"/>
       <c r="AD13" s="1">
         <v>42893</v>
@@ -1143,6 +1183,9 @@
       <c r="W15" s="1">
         <v>42874</v>
       </c>
+      <c r="X15" t="s">
+        <v>37</v>
+      </c>
       <c r="AC15" s="7"/>
       <c r="AD15" s="1">
         <v>42894</v>
@@ -1206,6 +1249,9 @@
       <c r="W17" s="1">
         <v>42877</v>
       </c>
+      <c r="X17" t="s">
+        <v>30</v>
+      </c>
       <c r="AC17" s="7"/>
       <c r="AD17" s="1">
         <v>42895</v>
@@ -1263,6 +1309,9 @@
       <c r="V19" s="7"/>
       <c r="W19" s="1">
         <v>42878</v>
+      </c>
+      <c r="X19" t="s">
+        <v>38</v>
       </c>
       <c r="AC19" s="7"/>
       <c r="AD19" s="1">

</xml_diff>

<commit_message>
Statistic Activity slightly updated Comments on my methods added
</commit_message>
<xml_diff>
--- a/documents/DailyScrums.xlsx
+++ b/documents/DailyScrums.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>1.Sprint</t>
   </si>
@@ -141,6 +141,15 @@
   </si>
   <si>
     <t>Sprint Review</t>
+  </si>
+  <si>
+    <t>Besprechung zur Spielverwaltung</t>
+  </si>
+  <si>
+    <t>Ist-Stand:</t>
+  </si>
+  <si>
+    <t>Sprintziel erreicht</t>
   </si>
 </sst>
 </file>
@@ -270,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -297,14 +306,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -620,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI22"/>
+  <dimension ref="A1:AJ25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AG13" sqref="AG13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25:N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,7 +651,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3">
@@ -670,13 +683,13 @@
       <c r="P1" s="3">
         <v>42851</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
       <c r="V1" s="6" t="s">
         <v>4</v>
       </c>
@@ -705,7 +718,7 @@
       <c r="AI1" s="9"/>
     </row>
     <row r="2" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
+      <c r="A2" s="12"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -742,7 +755,7 @@
       <c r="AI2" s="5"/>
     </row>
     <row r="3" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="1">
         <v>42810</v>
       </c>
@@ -774,9 +787,12 @@
       <c r="AD3" s="1">
         <v>42884</v>
       </c>
+      <c r="AE3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -813,7 +829,7 @@
       <c r="AI4" s="5"/>
     </row>
     <row r="5" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="1">
         <v>42811</v>
       </c>
@@ -845,9 +861,12 @@
       <c r="AD5" s="1">
         <v>42885</v>
       </c>
+      <c r="AE5" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="6" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -884,7 +903,7 @@
       <c r="AI6" s="5"/>
     </row>
     <row r="7" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="1">
         <v>42814</v>
       </c>
@@ -918,7 +937,7 @@
       </c>
     </row>
     <row r="8" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -955,7 +974,7 @@
       <c r="AI8" s="5"/>
     </row>
     <row r="9" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="1">
         <v>42815</v>
       </c>
@@ -989,7 +1008,7 @@
       </c>
     </row>
     <row r="10" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -1026,7 +1045,7 @@
       <c r="AI10" s="5"/>
     </row>
     <row r="11" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="1">
         <v>42816</v>
       </c>
@@ -1060,7 +1079,7 @@
       </c>
     </row>
     <row r="12" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1097,7 +1116,7 @@
       <c r="AI12" s="5"/>
     </row>
     <row r="13" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="1">
         <v>42817</v>
       </c>
@@ -1126,7 +1145,7 @@
       </c>
     </row>
     <row r="14" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1163,7 +1182,7 @@
       <c r="AI14" s="5"/>
     </row>
     <row r="15" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="1">
         <v>42818</v>
       </c>
@@ -1192,7 +1211,7 @@
       </c>
     </row>
     <row r="16" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -1228,8 +1247,8 @@
       <c r="AH16" s="5"/>
       <c r="AI16" s="5"/>
     </row>
-    <row r="17" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
+    <row r="17" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
       <c r="B17" s="1">
         <v>42821</v>
       </c>
@@ -1257,8 +1276,8 @@
         <v>42895</v>
       </c>
     </row>
-    <row r="18" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
+    <row r="18" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -1294,8 +1313,8 @@
       <c r="AH18" s="5"/>
       <c r="AI18" s="5"/>
     </row>
-    <row r="19" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
+    <row r="19" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
       <c r="B19" s="1">
         <v>42822</v>
       </c>
@@ -1318,8 +1337,8 @@
         <v>42898</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
+    <row r="20" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -1355,8 +1374,8 @@
       <c r="AH20" s="5"/>
       <c r="AI20" s="5"/>
     </row>
-    <row r="21" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+    <row r="21" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
       <c r="B21" s="1">
         <v>42823</v>
       </c>
@@ -1374,8 +1393,8 @@
         <v>42899</v>
       </c>
     </row>
-    <row r="22" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+    <row r="22" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -1411,8 +1430,107 @@
       <c r="AH22" s="5"/>
       <c r="AI22" s="5"/>
     </row>
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="I25" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
+      <c r="P25" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q25" s="14"/>
+      <c r="R25" s="14"/>
+      <c r="S25" s="14"/>
+      <c r="T25" s="14"/>
+      <c r="U25" s="14"/>
+      <c r="W25" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="X25" s="14"/>
+      <c r="Y25" s="14"/>
+      <c r="Z25" s="14"/>
+      <c r="AA25" s="14"/>
+      <c r="AB25" s="14"/>
+      <c r="AE25" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF25" s="14"/>
+      <c r="AG25" s="14"/>
+      <c r="AH25" s="14"/>
+      <c r="AI25" s="14"/>
+      <c r="AJ25" s="14"/>
+    </row>
   </sheetData>
-  <mergeCells count="65">
+  <mergeCells count="70">
+    <mergeCell ref="AE25:AJ25"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="I25:N25"/>
+    <mergeCell ref="P25:U25"/>
+    <mergeCell ref="W25:AB25"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="I4:N4"/>
+    <mergeCell ref="I6:N6"/>
+    <mergeCell ref="I8:N8"/>
+    <mergeCell ref="H1:H22"/>
+    <mergeCell ref="I22:N22"/>
+    <mergeCell ref="I10:N10"/>
+    <mergeCell ref="I12:N12"/>
+    <mergeCell ref="I14:N14"/>
+    <mergeCell ref="I16:N16"/>
+    <mergeCell ref="I18:N18"/>
+    <mergeCell ref="I20:N20"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="A1:A22"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="O1:O22"/>
+    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="P2:U2"/>
+    <mergeCell ref="P4:U4"/>
+    <mergeCell ref="P6:U6"/>
+    <mergeCell ref="P8:U8"/>
+    <mergeCell ref="P10:U10"/>
+    <mergeCell ref="P12:U12"/>
+    <mergeCell ref="P14:U14"/>
+    <mergeCell ref="P22:U22"/>
+    <mergeCell ref="P16:U16"/>
+    <mergeCell ref="P18:U18"/>
+    <mergeCell ref="P20:U20"/>
+    <mergeCell ref="V1:V22"/>
+    <mergeCell ref="X1:AB1"/>
+    <mergeCell ref="W2:AB2"/>
+    <mergeCell ref="W4:AB4"/>
+    <mergeCell ref="W6:AB6"/>
+    <mergeCell ref="W8:AB8"/>
+    <mergeCell ref="W14:AB14"/>
+    <mergeCell ref="W16:AB16"/>
+    <mergeCell ref="W18:AB18"/>
+    <mergeCell ref="W20:AB20"/>
     <mergeCell ref="AD16:AI16"/>
     <mergeCell ref="AD18:AI18"/>
     <mergeCell ref="AD20:AI20"/>
@@ -1429,57 +1547,8 @@
     <mergeCell ref="AD14:AI14"/>
     <mergeCell ref="W10:AB10"/>
     <mergeCell ref="W12:AB12"/>
-    <mergeCell ref="V1:V22"/>
-    <mergeCell ref="X1:AB1"/>
-    <mergeCell ref="W2:AB2"/>
-    <mergeCell ref="W4:AB4"/>
-    <mergeCell ref="W6:AB6"/>
-    <mergeCell ref="W8:AB8"/>
-    <mergeCell ref="W14:AB14"/>
-    <mergeCell ref="W16:AB16"/>
-    <mergeCell ref="W18:AB18"/>
-    <mergeCell ref="W20:AB20"/>
-    <mergeCell ref="O1:O22"/>
-    <mergeCell ref="Q1:U1"/>
-    <mergeCell ref="P2:U2"/>
-    <mergeCell ref="P4:U4"/>
-    <mergeCell ref="P6:U6"/>
-    <mergeCell ref="P8:U8"/>
-    <mergeCell ref="P10:U10"/>
-    <mergeCell ref="P12:U12"/>
-    <mergeCell ref="P14:U14"/>
-    <mergeCell ref="P22:U22"/>
-    <mergeCell ref="P16:U16"/>
-    <mergeCell ref="P18:U18"/>
-    <mergeCell ref="P20:U20"/>
-    <mergeCell ref="A1:A22"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B22:G22"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="I4:N4"/>
-    <mergeCell ref="I6:N6"/>
-    <mergeCell ref="I8:N8"/>
-    <mergeCell ref="H1:H22"/>
-    <mergeCell ref="I22:N22"/>
-    <mergeCell ref="I10:N10"/>
-    <mergeCell ref="I12:N12"/>
-    <mergeCell ref="I14:N14"/>
-    <mergeCell ref="I16:N16"/>
-    <mergeCell ref="I18:N18"/>
-    <mergeCell ref="I20:N20"/>
-    <mergeCell ref="J1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>